<commit_message>
Remove leading unnamed empty column that is irrelevant to this sheet's test usage
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/empty-named-column.xlsx
+++ b/tests/testthat/sheets/empty-named-column.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenny/rrr/readxl/tests/testthat/sheets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="600" windowWidth="27315" windowHeight="11505"/>
+    <workbookView xWindow="600" yWindow="600" windowWidth="27320" windowHeight="11500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -125,12 +136,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -160,12 +171,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -369,74 +380,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="E2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Use tibble::repair_names() to eliminate empty, NA, duplicated column names (#247)
* Remove leading unnamed empty column that is irrelevant to this sheet's test usage

* Use tibble::repair_names(); fixes #199, fixes #53

* Put a version on tibble and switch to as_tibble()
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/empty-named-column.xlsx
+++ b/tests/testthat/sheets/empty-named-column.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenny/rrr/readxl/tests/testthat/sheets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="600" windowWidth="27315" windowHeight="11505"/>
+    <workbookView xWindow="600" yWindow="600" windowWidth="27320" windowHeight="11500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -125,12 +136,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -160,12 +171,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -369,74 +380,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="E2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>